<commit_message>
committed till citizendhip but code is working
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/OPAS_TestData.xlsx
+++ b/src/main/java/testdata/OPAS_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6F833B-CBB5-4B73-9574-31B0CEC01998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6ABBF6-3C31-4505-8F3A-DC3C97BA0C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32880" yWindow="6090" windowWidth="21600" windowHeight="11295" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAS_SIT" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>FORM</t>
   </si>
@@ -102,12 +102,6 @@
     <t>FAMILYNAME</t>
   </si>
   <si>
-    <t>25 Burnum Burnum Cl, BONNER ACT 2914</t>
-  </si>
-  <si>
-    <t>RESEDENTIAL ADDRESS</t>
-  </si>
-  <si>
     <t>RESIDENCE COUNTRY</t>
   </si>
   <si>
@@ -175,6 +169,30 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>10/05/1985</t>
+  </si>
+  <si>
+    <t>RESEDENTIALADDRESSINE1</t>
+  </si>
+  <si>
+    <t>SUBURB</t>
+  </si>
+  <si>
+    <t>POSTCODE</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
+  <si>
+    <t>ACT</t>
+  </si>
+  <si>
+    <t>25 Burnum Burnum Cl</t>
+  </si>
+  <si>
+    <t>BONNER</t>
   </si>
 </sst>
 </file>
@@ -222,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -232,6 +250,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -548,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E58059-435B-46A4-A352-82E5087E05D1}">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,22 +585,23 @@
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
     <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" customWidth="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.140625" customWidth="1"/>
-    <col min="22" max="23" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.5703125" customWidth="1"/>
-    <col min="25" max="25" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="37.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" customWidth="1"/>
+    <col min="25" max="26" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.5703125" customWidth="1"/>
+    <col min="28" max="28" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -620,59 +642,68 @@
         <v>8</v>
       </c>
       <c r="N1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="X1" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" s="5"/>
+      <c r="AH1" s="5"/>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -714,7 +745,7 @@
       </c>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -728,19 +759,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
         <v>42</v>
       </c>
-      <c r="G3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="6">
-        <v>31204</v>
+      <c r="H3" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
         <v>14</v>
@@ -755,43 +786,52 @@
         <v>44742</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O3" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3">
+        <v>2914</v>
+      </c>
+      <c r="S3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" s="2">
+        <v>31204</v>
+      </c>
+      <c r="V3">
+        <v>2145507795</v>
+      </c>
+      <c r="W3" s="2">
+        <v>43230</v>
+      </c>
+      <c r="X3" s="2">
+        <v>43230</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R3" s="2">
+      <c r="AA3" s="6">
         <v>31204</v>
       </c>
-      <c r="S3">
-        <v>2145507795</v>
-      </c>
-      <c r="T3" s="2">
-        <v>43230</v>
-      </c>
-      <c r="U3" s="2">
-        <v>43230</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="X3" s="6">
-        <v>31204</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>37</v>
+      <c r="AB3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
committed with end to end code working
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/OPAS_TestData.xlsx
+++ b/src/main/java/testdata/OPAS_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6ABBF6-3C31-4505-8F3A-DC3C97BA0C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2CE16D-E7B8-442C-B1B4-E23371A04549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
+    <workbookView xWindow="34110" yWindow="2940" windowWidth="21600" windowHeight="12645" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
   </bookViews>
   <sheets>
     <sheet name="OPAS_SIT" sheetId="1" r:id="rId1"/>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E58059-435B-46A4-A352-82E5087E05D1}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
committed with end to end data working and Excel update
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/OPAS_TestData.xlsx
+++ b/src/main/java/testdata/OPAS_TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CD7A05-6E68-4E3C-A97F-B792960B4CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FDA449-39C1-4EDC-A13B-15A8F37D10A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>FORM</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>FormNumber</t>
+  </si>
+  <si>
+    <t>S14523075</t>
   </si>
 </sst>
 </file>
@@ -527,26 +530,26 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="25" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -621,6 +624,9 @@
       <c r="A2" t="s">
         <v>17</v>
       </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
@@ -657,7 +663,6 @@
       <c r="N2" s="2">
         <v>44742</v>
       </c>
-      <c r="R2" s="2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">

</xml_diff>

<commit_message>
commited with application number printing
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/OPAS_TestData.xlsx
+++ b/src/main/java/testdata/OPAS_TestData.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21701F2B-29BA-461F-82BE-A51C8F53575F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{45B99322-3D49-4C56-8356-F8DC250439D4}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}"/>
+    <workbookView activeTab="1" windowHeight="13020" windowWidth="24240" xWindow="28680" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="PC1_CitizenshipCertificate" sheetId="1" r:id="rId1"/>
-    <sheet name="PC7_PassportRenewal" sheetId="2" r:id="rId2"/>
+    <sheet name="PC1_CitizenshipCertificate" r:id="rId1" sheetId="1"/>
+    <sheet name="PC7_PassportRenewal" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="51">
   <si>
     <t>FORM</t>
   </si>
@@ -194,6 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,26 +234,26 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -269,10 +270,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -307,7 +308,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -359,7 +360,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -470,21 +471,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -501,7 +502,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -553,37 +554,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E58059-435B-46A4-A352-82E5087E05D1}">
-  <dimension ref="A1:V3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E58059-435B-46A4-A352-82E5087E05D1}">
+  <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="25" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="6.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="25.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -697,10 +698,21 @@
       <c r="N2" s="2">
         <v>44742</v>
       </c>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -763,28 +775,226 @@
         <v>2914</v>
       </c>
     </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4">
+        <v>1690509279</v>
+      </c>
+      <c r="N4" s="2">
+        <v>44742</v>
+      </c>
+      <c r="O4">
+        <v>2145507795</v>
+      </c>
+      <c r="P4" s="2">
+        <v>43230</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>43230</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5">
+        <v>1690509279</v>
+      </c>
+      <c r="N5" s="2">
+        <v>44742</v>
+      </c>
+      <c r="O5">
+        <v>2145507795</v>
+      </c>
+      <c r="P5" s="2">
+        <v>43230</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>43230</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S5" t="s">
+        <v>36</v>
+      </c>
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6">
+        <v>1690509279</v>
+      </c>
+      <c r="N6" s="2">
+        <v>44742</v>
+      </c>
+      <c r="O6">
+        <v>2145507795</v>
+      </c>
+      <c r="P6" s="2">
+        <v>43230</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>43230</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" t="s">
+        <v>37</v>
+      </c>
+      <c r="U6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6">
+        <v>2914</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C4AA5D-90B4-4B28-90DA-A8012B3348DF}">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C4AA5D-90B4-4B28-90DA-A8012B3348DF}">
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -904,7 +1114,130 @@
         <v>44448</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2">
+        <v>40795</v>
+      </c>
+      <c r="N4" s="2">
+        <v>44448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="3">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5" s="2">
+        <v>40795</v>
+      </c>
+      <c r="N5" s="2">
+        <v>44448</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M6" s="2">
+        <v>40795</v>
+      </c>
+      <c r="N6" s="2">
+        <v>44448</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
committed on 06 Dec
</commit_message>
<xml_diff>
--- a/src/main/java/testdata/OPAS_TestData.xlsx
+++ b/src/main/java/testdata/OPAS_TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanpr\exlipsefolder2\DFAT_PassportProject\src\main\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7556CB02-CB41-43A4-8A36-C2C7CA617867}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{78CD1D14-70AC-4CAB-83D5-E2DE56C6FD83}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView windowHeight="13020" windowWidth="24240" xWindow="28680" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}" yWindow="-120"/>
+    <workbookView activeTab="1" windowHeight="13020" windowWidth="24240" xWindow="28680" xr2:uid="{84FAEEE2-7639-48EA-AA82-76271FAE16F1}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="PC1_CitizenshipCertificate" r:id="rId1" sheetId="1"/>
     <sheet name="PC7_PassportRenewal" r:id="rId2" sheetId="2"/>
+    <sheet name="PC1_BirthCertificate" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="68">
   <si>
     <t>FORM</t>
   </si>
@@ -163,31 +164,82 @@
     <t>ISSUEDATE</t>
   </si>
   <si>
+    <t>Meegan Edwina</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>EXPIRYDATE</t>
+  </si>
+  <si>
+    <t>27/09/1988</t>
+  </si>
+  <si>
+    <t>PREVIOUSPASSPORTNUMBER</t>
+  </si>
+  <si>
+    <t>06/06/1985</t>
+  </si>
+  <si>
+    <t>S1475860</t>
+  </si>
+  <si>
+    <t>Remi</t>
+  </si>
+  <si>
+    <t>Nishiura</t>
+  </si>
+  <si>
+    <t>31/05/1997</t>
+  </si>
+  <si>
+    <t>Paddington</t>
+  </si>
+  <si>
+    <t>BirthCe</t>
+  </si>
+  <si>
+    <t>CITIZENSHIP</t>
+  </si>
+  <si>
+    <t>40012/1997</t>
+  </si>
+  <si>
     <t>Argent</t>
   </si>
   <si>
-    <t>Meegan Edwina</t>
-  </si>
-  <si>
-    <t>Sydney</t>
-  </si>
-  <si>
-    <t>Australia</t>
-  </si>
-  <si>
-    <t>EXPIRYDATE</t>
-  </si>
-  <si>
-    <t>27/09/1988</t>
-  </si>
-  <si>
-    <t>PREVIOUSPASSPORTNUMBER</t>
-  </si>
-  <si>
-    <t>06/06/1985</t>
-  </si>
-  <si>
-    <t>S1475860</t>
+    <t>BIRTH_CERTIFICATE_NUMBER</t>
+  </si>
+  <si>
+    <t>BIRTH_CERTIFICATE_ISSUEDATE</t>
+  </si>
+  <si>
+    <t>DATE_ISSUED</t>
+  </si>
+  <si>
+    <t>BIRTH_CERTIFICATE_REGISTERED_DATE</t>
+  </si>
+  <si>
+    <t>BIRTHCERTIFICATEISSUESTATE</t>
+  </si>
+  <si>
+    <t>NSW</t>
+  </si>
+  <si>
+    <t>28/01/2016</t>
+  </si>
+  <si>
+    <t>8/07/1997</t>
+  </si>
+  <si>
+    <t>24/06/1997</t>
+  </si>
+  <si>
+    <t>10/05/2018</t>
   </si>
 </sst>
 </file>
@@ -195,10 +247,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" xfId="0"/>
@@ -248,6 +306,7 @@
     <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="14" quotePrefix="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -564,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01E58059-435B-46A4-A352-82E5087E05D1}">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:B3"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,7 +771,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3">
         <v>2</v>
@@ -733,7 +792,7 @@
         <v>30</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J3" t="s">
         <v>27</v>
@@ -777,9 +836,11 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4"/>
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
       <c r="C4" s="3">
         <v>3</v>
       </c>
@@ -799,7 +860,7 @@
         <v>30</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
         <v>27</v>
@@ -843,9 +904,11 @@
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5"/>
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
@@ -865,7 +928,7 @@
         <v>30</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J5" t="s">
         <v>27</v>
@@ -909,9 +972,11 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6"/>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -931,7 +996,7 @@
         <v>30</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J6" t="s">
         <v>27</v>
@@ -983,12 +1048,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C4AA5D-90B4-4B28-90DA-A8012B3348DF}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" customWidth="true" width="17.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
@@ -1032,13 +1098,13 @@
         <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1056,7 +1122,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -1079,11 +1145,9 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B3"/>
       <c r="C3" s="3">
         <v>2</v>
       </c>
@@ -1092,22 +1156,22 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" t="s">
         <v>42</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
       </c>
       <c r="H3" t="s">
         <v>30</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="s">
         <v>44</v>
-      </c>
-      <c r="K3" t="s">
-        <v>45</v>
       </c>
       <c r="L3" t="s">
         <v>40</v>
@@ -1132,22 +1196,22 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" t="s">
         <v>42</v>
-      </c>
-      <c r="G4" t="s">
-        <v>43</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
         <v>44</v>
-      </c>
-      <c r="K4" t="s">
-        <v>45</v>
       </c>
       <c r="L4" t="s">
         <v>40</v>
@@ -1161,9 +1225,11 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5"/>
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
@@ -1172,22 +1238,22 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
         <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>45</v>
       </c>
       <c r="L5" t="s">
         <v>40</v>
@@ -1201,9 +1267,11 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6"/>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
@@ -1212,22 +1280,22 @@
         <v>7</v>
       </c>
       <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
         <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>43</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" t="s">
         <v>44</v>
-      </c>
-      <c r="K6" t="s">
-        <v>45</v>
       </c>
       <c r="L6" t="s">
         <v>40</v>
@@ -1238,6 +1306,225 @@
       <c r="N6" s="2">
         <v>44448</v>
       </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3866F1-0712-43CC-A03A-0F030F499417}">
+  <dimension ref="A1:W6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="4">
+        <v>31907</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2">
+        <v>1690509279</v>
+      </c>
+      <c r="N2" s="2">
+        <v>44742</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M3">
+        <v>1690509279</v>
+      </c>
+      <c r="N3" s="2">
+        <v>44742</v>
+      </c>
+      <c r="O3">
+        <v>30505941</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>